<commit_message>
Added Go and Rust, got data for Go done
</commit_message>
<xml_diff>
--- a/ExperimentParameters.xlsx
+++ b/ExperimentParameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monkj\CS630Project\CS630Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55CEDAE-41A0-485B-8077-4EB4E35E0FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54AEFB8-F663-4AB2-A1E3-D53A28BAA059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="33">
   <si>
     <t>Languages</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Trial 10</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>Rust</t>
   </si>
 </sst>
 </file>
@@ -384,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -394,6 +400,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -406,6 +419,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -415,20 +434,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -712,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,31 +742,31 @@
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="12"/>
+      <c r="H2" s="17"/>
       <c r="L2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -784,8 +789,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2">
@@ -814,8 +819,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="2">
@@ -841,8 +846,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="2">
@@ -871,8 +876,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="2">
@@ -898,8 +903,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="2">
@@ -925,8 +930,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="2">
@@ -955,8 +960,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="2">
@@ -988,8 +993,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="2">
@@ -1018,8 +1023,8 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="2">
@@ -1045,8 +1050,8 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="20" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="3">
@@ -1072,40 +1077,40 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="1">
-        <f>AVERAGE(C4:C13)</f>
+        <f t="shared" ref="C14:H14" si="0">AVERAGE(C4:C13)</f>
         <v>1.4382999999999999</v>
       </c>
-      <c r="D14" s="23">
-        <f>AVERAGE(D4:D13)</f>
+      <c r="D14" s="13">
+        <f t="shared" si="0"/>
         <v>28.25</v>
       </c>
-      <c r="E14" s="22">
-        <f>AVERAGE(E4:E13)</f>
+      <c r="E14" s="12">
+        <f t="shared" si="0"/>
         <v>7.8882999999999992</v>
       </c>
-      <c r="F14" s="23">
-        <f>AVERAGE(F4:F13)</f>
+      <c r="F14" s="13">
+        <f t="shared" si="0"/>
         <v>43.23</v>
       </c>
-      <c r="G14" s="22">
-        <f>AVERAGE(G4:G13)</f>
+      <c r="G14" s="12">
+        <f t="shared" si="0"/>
         <v>15.535900000000002</v>
       </c>
-      <c r="H14" s="23">
-        <f>AVERAGE(H4:H13)</f>
+      <c r="H14" s="13">
+        <f t="shared" si="0"/>
         <v>42.409999999999989</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -1128,8 +1133,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="2">
@@ -1155,8 +1160,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="2">
@@ -1182,8 +1187,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="19" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="2">
@@ -1209,8 +1214,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="19" t="s">
+      <c r="A19" s="21"/>
+      <c r="B19" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="2">
@@ -1236,8 +1241,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="21"/>
+      <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="2">
@@ -1263,8 +1268,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="19" t="s">
+      <c r="A21" s="21"/>
+      <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="2">
@@ -1290,8 +1295,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="19" t="s">
+      <c r="A22" s="21"/>
+      <c r="B22" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="2">
@@ -1317,8 +1322,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="19" t="s">
+      <c r="A23" s="21"/>
+      <c r="B23" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="2">
@@ -1344,8 +1349,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="19" t="s">
+      <c r="A24" s="21"/>
+      <c r="B24" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="2">
@@ -1371,8 +1376,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="20" t="s">
+      <c r="A25" s="21"/>
+      <c r="B25" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="3">
@@ -1398,40 +1403,40 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="1">
-        <f>AVERAGE(C16:C25)</f>
+        <f t="shared" ref="C26:H26" si="1">AVERAGE(C16:C25)</f>
         <v>0.20850000000000005</v>
       </c>
-      <c r="D26" s="23">
-        <f>AVERAGE(D16:D25)</f>
+      <c r="D26" s="13">
+        <f t="shared" si="1"/>
         <v>24.03</v>
       </c>
-      <c r="E26" s="22">
-        <f>AVERAGE(E16:E25)</f>
+      <c r="E26" s="12">
+        <f t="shared" si="1"/>
         <v>2.4047000000000001</v>
       </c>
-      <c r="F26" s="23">
-        <f>AVERAGE(F16:F25)</f>
+      <c r="F26" s="13">
+        <f t="shared" si="1"/>
         <v>43.290000000000006</v>
       </c>
-      <c r="G26" s="22">
-        <f>AVERAGE(G16:G25)</f>
+      <c r="G26" s="12">
+        <f t="shared" si="1"/>
         <v>33.483500000000006</v>
       </c>
-      <c r="H26" s="23">
-        <f>AVERAGE(H16:H25)</f>
+      <c r="H26" s="13">
+        <f t="shared" si="1"/>
         <v>43.510000000000005</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="8" t="s">
@@ -1454,8 +1459,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="19" t="s">
+      <c r="A28" s="21"/>
+      <c r="B28" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="2">
@@ -1481,8 +1486,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="19" t="s">
+      <c r="A29" s="21"/>
+      <c r="B29" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="2">
@@ -1508,8 +1513,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="19" t="s">
+      <c r="A30" s="21"/>
+      <c r="B30" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="2">
@@ -1535,8 +1540,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="19" t="s">
+      <c r="A31" s="21"/>
+      <c r="B31" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="2">
@@ -1562,8 +1567,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="19" t="s">
+      <c r="A32" s="21"/>
+      <c r="B32" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="2">
@@ -1589,8 +1594,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="19" t="s">
+      <c r="A33" s="21"/>
+      <c r="B33" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="2">
@@ -1616,8 +1621,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="19" t="s">
+      <c r="A34" s="21"/>
+      <c r="B34" t="s">
         <v>27</v>
       </c>
       <c r="C34" s="2">
@@ -1643,8 +1648,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="19" t="s">
+      <c r="A35" s="21"/>
+      <c r="B35" t="s">
         <v>28</v>
       </c>
       <c r="C35" s="2">
@@ -1670,8 +1675,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="19" t="s">
+      <c r="A36" s="21"/>
+      <c r="B36" t="s">
         <v>29</v>
       </c>
       <c r="C36" s="2">
@@ -1697,8 +1702,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="20" t="s">
+      <c r="A37" s="21"/>
+      <c r="B37" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="3">
@@ -1724,40 +1729,40 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C38" s="1">
-        <f>AVERAGE(C28:C37)</f>
+        <f t="shared" ref="C38:H38" si="2">AVERAGE(C28:C37)</f>
         <v>0.39339999999999997</v>
       </c>
-      <c r="D38" s="23">
-        <f>AVERAGE(D28:D37)</f>
+      <c r="D38" s="13">
+        <f t="shared" si="2"/>
         <v>25.630000000000006</v>
       </c>
-      <c r="E38" s="22">
-        <f>AVERAGE(E28:E37)</f>
+      <c r="E38" s="12">
+        <f t="shared" si="2"/>
         <v>6.4282999999999983</v>
       </c>
-      <c r="F38" s="23">
-        <f>AVERAGE(F28:F37)</f>
+      <c r="F38" s="13">
+        <f t="shared" si="2"/>
         <v>38.660000000000011</v>
       </c>
-      <c r="G38" s="22">
-        <f>AVERAGE(G28:G37)</f>
+      <c r="G38" s="12">
+        <f t="shared" si="2"/>
         <v>44.493100000000005</v>
       </c>
-      <c r="H38" s="23">
-        <f>AVERAGE(H28:H37)</f>
+      <c r="H38" s="13">
+        <f t="shared" si="2"/>
         <v>39.109999999999992</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -1780,8 +1785,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="19" t="s">
+      <c r="A40" s="21"/>
+      <c r="B40" t="s">
         <v>21</v>
       </c>
       <c r="C40" s="2">
@@ -1802,8 +1807,8 @@
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="19" t="s">
+      <c r="A41" s="21"/>
+      <c r="B41" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="2">
@@ -1824,8 +1829,8 @@
       <c r="H41" s="6"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="19" t="s">
+      <c r="A42" s="21"/>
+      <c r="B42" t="s">
         <v>23</v>
       </c>
       <c r="C42" s="2">
@@ -1841,8 +1846,8 @@
       <c r="H42" s="6"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="19" t="s">
+      <c r="A43" s="21"/>
+      <c r="B43" t="s">
         <v>24</v>
       </c>
       <c r="C43" s="2">
@@ -1858,8 +1863,8 @@
       <c r="H43" s="6"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="19" t="s">
+      <c r="A44" s="21"/>
+      <c r="B44" t="s">
         <v>25</v>
       </c>
       <c r="C44" s="2">
@@ -1875,8 +1880,8 @@
       <c r="H44" s="6"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="19" t="s">
+      <c r="A45" s="21"/>
+      <c r="B45" t="s">
         <v>26</v>
       </c>
       <c r="C45" s="2">
@@ -1892,8 +1897,8 @@
       <c r="H45" s="6"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="19" t="s">
+      <c r="A46" s="21"/>
+      <c r="B46" t="s">
         <v>27</v>
       </c>
       <c r="C46" s="2">
@@ -1909,8 +1914,8 @@
       <c r="H46" s="6"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="19" t="s">
+      <c r="A47" s="21"/>
+      <c r="B47" t="s">
         <v>28</v>
       </c>
       <c r="C47" s="2">
@@ -1926,8 +1931,8 @@
       <c r="H47" s="6"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="19" t="s">
+      <c r="A48" s="21"/>
+      <c r="B48" t="s">
         <v>29</v>
       </c>
       <c r="C48" s="2">
@@ -1943,8 +1948,8 @@
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="14"/>
-      <c r="B49" s="20" t="s">
+      <c r="A49" s="21"/>
+      <c r="B49" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C49" s="3">
@@ -1960,7 +1965,7 @@
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="15"/>
+      <c r="A50" s="22"/>
       <c r="B50" s="8" t="s">
         <v>20</v>
       </c>
@@ -1968,20 +1973,20 @@
         <f>AVERAGE(C40:C49)</f>
         <v>18.398500000000002</v>
       </c>
-      <c r="D50" s="23">
+      <c r="D50" s="13">
         <f>AVERAGE(D40:D49)</f>
         <v>51.4</v>
       </c>
-      <c r="E50" s="22"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="23"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C51" s="8" t="s">
@@ -2004,8 +2009,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="19" t="s">
+      <c r="A52" s="21"/>
+      <c r="B52" t="s">
         <v>21</v>
       </c>
       <c r="C52" s="2">
@@ -2031,8 +2036,8 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="19" t="s">
+      <c r="A53" s="21"/>
+      <c r="B53" t="s">
         <v>22</v>
       </c>
       <c r="C53" s="2">
@@ -2058,8 +2063,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="19" t="s">
+      <c r="A54" s="21"/>
+      <c r="B54" t="s">
         <v>23</v>
       </c>
       <c r="C54" s="2">
@@ -2085,8 +2090,8 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
-      <c r="B55" s="19" t="s">
+      <c r="A55" s="21"/>
+      <c r="B55" t="s">
         <v>24</v>
       </c>
       <c r="C55" s="2">
@@ -2112,8 +2117,8 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="19" t="s">
+      <c r="A56" s="21"/>
+      <c r="B56" t="s">
         <v>25</v>
       </c>
       <c r="C56" s="2">
@@ -2139,8 +2144,8 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
-      <c r="B57" s="19" t="s">
+      <c r="A57" s="21"/>
+      <c r="B57" t="s">
         <v>26</v>
       </c>
       <c r="C57" s="2">
@@ -2166,8 +2171,8 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="19" t="s">
+      <c r="A58" s="21"/>
+      <c r="B58" t="s">
         <v>27</v>
       </c>
       <c r="C58" s="2">
@@ -2193,8 +2198,8 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="19" t="s">
+      <c r="A59" s="21"/>
+      <c r="B59" t="s">
         <v>28</v>
       </c>
       <c r="C59" s="2">
@@ -2220,8 +2225,8 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="19" t="s">
+      <c r="A60" s="21"/>
+      <c r="B60" t="s">
         <v>29</v>
       </c>
       <c r="C60" s="2">
@@ -2247,8 +2252,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="14"/>
-      <c r="B61" s="20" t="s">
+      <c r="A61" s="21"/>
+      <c r="B61" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C61" s="3">
@@ -2274,40 +2279,40 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="24"/>
+      <c r="A62" s="23"/>
       <c r="B62" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C62" s="1">
-        <f>AVERAGE(C52:C61)</f>
+        <f t="shared" ref="C62:H62" si="3">AVERAGE(C52:C61)</f>
         <v>1.4441000000000002</v>
       </c>
-      <c r="D62" s="23">
-        <f>AVERAGE(D52:D61)</f>
+      <c r="D62" s="13">
+        <f t="shared" si="3"/>
         <v>28.24</v>
       </c>
-      <c r="E62" s="22">
-        <f>AVERAGE(E52:E61)</f>
+      <c r="E62" s="12">
+        <f t="shared" si="3"/>
         <v>7.5444000000000013</v>
       </c>
-      <c r="F62" s="23">
-        <f>AVERAGE(F52:F61)</f>
+      <c r="F62" s="13">
+        <f t="shared" si="3"/>
         <v>42.849999999999994</v>
       </c>
-      <c r="G62" s="22">
-        <f>AVERAGE(G52:G61)</f>
+      <c r="G62" s="12">
+        <f t="shared" si="3"/>
         <v>16.2332</v>
       </c>
-      <c r="H62" s="23">
-        <f>AVERAGE(H52:H61)</f>
+      <c r="H62" s="13">
+        <f t="shared" si="3"/>
         <v>40.43</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B63" s="18" t="s">
+      <c r="B63" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C63" s="8" t="s">
@@ -2330,8 +2335,8 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
-      <c r="B64" s="19" t="s">
+      <c r="A64" s="21"/>
+      <c r="B64" t="s">
         <v>21</v>
       </c>
       <c r="C64" s="2">
@@ -2357,8 +2362,8 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="19" t="s">
+      <c r="A65" s="21"/>
+      <c r="B65" t="s">
         <v>22</v>
       </c>
       <c r="C65" s="2">
@@ -2384,8 +2389,8 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="19" t="s">
+      <c r="A66" s="21"/>
+      <c r="B66" t="s">
         <v>23</v>
       </c>
       <c r="C66" s="2">
@@ -2411,8 +2416,8 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
-      <c r="B67" s="19" t="s">
+      <c r="A67" s="21"/>
+      <c r="B67" t="s">
         <v>24</v>
       </c>
       <c r="C67" s="2">
@@ -2438,8 +2443,8 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
-      <c r="B68" s="19" t="s">
+      <c r="A68" s="21"/>
+      <c r="B68" t="s">
         <v>25</v>
       </c>
       <c r="C68" s="2">
@@ -2465,8 +2470,8 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="19" t="s">
+      <c r="A69" s="21"/>
+      <c r="B69" t="s">
         <v>26</v>
       </c>
       <c r="C69" s="2">
@@ -2492,8 +2497,8 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
-      <c r="B70" s="19" t="s">
+      <c r="A70" s="21"/>
+      <c r="B70" t="s">
         <v>27</v>
       </c>
       <c r="C70" s="2">
@@ -2519,8 +2524,8 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
-      <c r="B71" s="19" t="s">
+      <c r="A71" s="21"/>
+      <c r="B71" t="s">
         <v>28</v>
       </c>
       <c r="C71" s="2">
@@ -2546,8 +2551,8 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
-      <c r="B72" s="19" t="s">
+      <c r="A72" s="21"/>
+      <c r="B72" t="s">
         <v>29</v>
       </c>
       <c r="C72" s="2">
@@ -2573,8 +2578,8 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="14"/>
-      <c r="B73" s="20" t="s">
+      <c r="A73" s="21"/>
+      <c r="B73" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C73" s="3">
@@ -2600,46 +2605,532 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="15"/>
+      <c r="A74" s="22"/>
       <c r="B74" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C74" s="1">
-        <f>AVERAGE(C64:C73)</f>
+        <f t="shared" ref="C74:H74" si="4">AVERAGE(C64:C73)</f>
         <v>0.5845999999999999</v>
       </c>
-      <c r="D74" s="23">
-        <f>AVERAGE(D64:D73)</f>
+      <c r="D74" s="13">
+        <f t="shared" si="4"/>
         <v>41.339999999999996</v>
       </c>
-      <c r="E74" s="22">
-        <f>AVERAGE(E64:E73)</f>
+      <c r="E74" s="12">
+        <f t="shared" si="4"/>
         <v>14.087700000000002</v>
       </c>
-      <c r="F74" s="23">
-        <f>AVERAGE(F64:F73)</f>
+      <c r="F74" s="13">
+        <f t="shared" si="4"/>
         <v>53.570000000000007</v>
       </c>
-      <c r="G74" s="22">
-        <f>AVERAGE(G64:G73)</f>
+      <c r="G74" s="12">
+        <f t="shared" si="4"/>
         <v>25.875800000000005</v>
       </c>
-      <c r="H74" s="23">
-        <f>AVERAGE(H64:H73)</f>
+      <c r="H74" s="13">
+        <f t="shared" si="4"/>
         <v>40.209999999999994</v>
       </c>
     </row>
+    <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F75" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H75" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="21"/>
+      <c r="B76" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="D76" s="5">
+        <f>73.4-L10</f>
+        <v>15.400000000000006</v>
+      </c>
+      <c r="E76" s="2">
+        <v>17.588999999999999</v>
+      </c>
+      <c r="F76" s="5">
+        <f>120.3-L10</f>
+        <v>62.3</v>
+      </c>
+      <c r="G76" s="2">
+        <v>38.594000000000001</v>
+      </c>
+      <c r="H76" s="5">
+        <f>109.2-L10</f>
+        <v>51.2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="21"/>
+      <c r="B77" t="s">
+        <v>22</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="D77" s="6">
+        <f>77.2-L10</f>
+        <v>19.200000000000003</v>
+      </c>
+      <c r="E77" s="2">
+        <v>17.193000000000001</v>
+      </c>
+      <c r="F77" s="6">
+        <f>116.7-L10</f>
+        <v>58.7</v>
+      </c>
+      <c r="G77" s="2">
+        <v>24.814</v>
+      </c>
+      <c r="H77" s="6">
+        <f>115.1-L10</f>
+        <v>57.099999999999994</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="21"/>
+      <c r="B78" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" s="2">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="D78" s="6">
+        <f>71-L10</f>
+        <v>13</v>
+      </c>
+      <c r="E78" s="2">
+        <v>17.146999999999998</v>
+      </c>
+      <c r="F78" s="6">
+        <f>126.8-L10</f>
+        <v>68.8</v>
+      </c>
+      <c r="G78" s="2">
+        <v>24.978999999999999</v>
+      </c>
+      <c r="H78" s="6">
+        <f>97.8-L10</f>
+        <v>39.799999999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+      <c r="B79" t="s">
+        <v>24</v>
+      </c>
+      <c r="C79" s="2">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="D79" s="6">
+        <f>78.3-L10</f>
+        <v>20.299999999999997</v>
+      </c>
+      <c r="E79" s="2">
+        <v>17.334</v>
+      </c>
+      <c r="F79" s="6">
+        <f>118.3-L10</f>
+        <v>60.3</v>
+      </c>
+      <c r="G79" s="2">
+        <v>24.962</v>
+      </c>
+      <c r="H79" s="6">
+        <f>94-L10</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="21"/>
+      <c r="B80" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="2">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="D80" s="6">
+        <f>72.5-L10</f>
+        <v>14.5</v>
+      </c>
+      <c r="E80" s="2">
+        <v>17.395</v>
+      </c>
+      <c r="F80" s="6">
+        <f>120.2-L10</f>
+        <v>62.2</v>
+      </c>
+      <c r="G80" s="2">
+        <v>25.407</v>
+      </c>
+      <c r="H80" s="6">
+        <f>95.6-L10</f>
+        <v>37.599999999999994</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="21"/>
+      <c r="B81" t="s">
+        <v>26</v>
+      </c>
+      <c r="C81" s="2">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="D81" s="6">
+        <f>74.6-L10</f>
+        <v>16.599999999999994</v>
+      </c>
+      <c r="E81" s="2">
+        <v>17.291</v>
+      </c>
+      <c r="F81" s="6">
+        <f>128.5-L10</f>
+        <v>70.5</v>
+      </c>
+      <c r="G81" s="2">
+        <v>25.222999999999999</v>
+      </c>
+      <c r="H81" s="6">
+        <f>94.2-L10</f>
+        <v>36.200000000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="21"/>
+      <c r="B82" t="s">
+        <v>27</v>
+      </c>
+      <c r="C82" s="2">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="D82" s="6">
+        <f>72.7-L10</f>
+        <v>14.700000000000003</v>
+      </c>
+      <c r="E82" s="2">
+        <v>17.263000000000002</v>
+      </c>
+      <c r="F82" s="6">
+        <f>119.9-L10</f>
+        <v>61.900000000000006</v>
+      </c>
+      <c r="G82" s="2">
+        <v>25.225999999999999</v>
+      </c>
+      <c r="H82" s="6">
+        <f>93.9-L10</f>
+        <v>35.900000000000006</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="21"/>
+      <c r="B83" t="s">
+        <v>28</v>
+      </c>
+      <c r="C83" s="2">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="D83" s="6">
+        <f>74.1-L10</f>
+        <v>16.099999999999994</v>
+      </c>
+      <c r="E83" s="2">
+        <v>17.321999999999999</v>
+      </c>
+      <c r="F83" s="6">
+        <f>122.6-L10</f>
+        <v>64.599999999999994</v>
+      </c>
+      <c r="G83" s="2">
+        <v>24.625</v>
+      </c>
+      <c r="H83" s="6">
+        <f>97.9-L10</f>
+        <v>39.900000000000006</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="21"/>
+      <c r="B84" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" s="2">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="D84" s="6">
+        <f>74.9-L10</f>
+        <v>16.900000000000006</v>
+      </c>
+      <c r="E84" s="2">
+        <v>16.768999999999998</v>
+      </c>
+      <c r="F84" s="6">
+        <f>119-L10</f>
+        <v>61</v>
+      </c>
+      <c r="G84" s="2">
+        <v>25.053000000000001</v>
+      </c>
+      <c r="H84" s="6">
+        <f>113.7-L10</f>
+        <v>55.7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="21"/>
+      <c r="B85" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" s="3">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="D85" s="7">
+        <f>74.4-L10</f>
+        <v>16.400000000000006</v>
+      </c>
+      <c r="E85" s="3">
+        <v>17.097000000000001</v>
+      </c>
+      <c r="F85" s="7">
+        <f>121-L10</f>
+        <v>63</v>
+      </c>
+      <c r="G85" s="3">
+        <v>24.827999999999999</v>
+      </c>
+      <c r="H85" s="7">
+        <f>113.1-L10</f>
+        <v>55.099999999999994</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="22"/>
+      <c r="B86" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86" s="1">
+        <f>AVERAGE(C76:C85)</f>
+        <v>0.19650000000000004</v>
+      </c>
+      <c r="D86" s="13">
+        <f>AVERAGE(D76:D85)</f>
+        <v>16.310000000000002</v>
+      </c>
+      <c r="E86" s="12">
+        <f>AVERAGE(E76:E85)</f>
+        <v>17.240000000000002</v>
+      </c>
+      <c r="F86" s="13">
+        <f>AVERAGE(F76:F85)</f>
+        <v>63.330000000000005</v>
+      </c>
+      <c r="G86" s="12">
+        <f>AVERAGE(G76:G85)</f>
+        <v>26.371099999999995</v>
+      </c>
+      <c r="H86" s="13">
+        <f>AVERAGE(H76:H85)</f>
+        <v>44.449999999999989</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E87" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H87" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="21"/>
+      <c r="B88" t="s">
+        <v>21</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="21"/>
+      <c r="B89" t="s">
+        <v>22</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="6"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="21"/>
+      <c r="B90" t="s">
+        <v>23</v>
+      </c>
+      <c r="C90" s="2"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="6"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="21"/>
+      <c r="B91" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="6"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="21"/>
+      <c r="B92" t="s">
+        <v>25</v>
+      </c>
+      <c r="C92" s="2"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="6"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="21"/>
+      <c r="B93" t="s">
+        <v>26</v>
+      </c>
+      <c r="C93" s="2"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="6"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="21"/>
+      <c r="B94" t="s">
+        <v>27</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="6"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="21"/>
+      <c r="B95" t="s">
+        <v>28</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="6"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="21"/>
+      <c r="B96" t="s">
+        <v>29</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="6"/>
+    </row>
+    <row r="97" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="21"/>
+      <c r="B97" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C97" s="3"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="7"/>
+    </row>
+    <row r="98" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="22"/>
+      <c r="B98" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C98" s="1"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="A87:A98"/>
+    <mergeCell ref="A27:A38"/>
+    <mergeCell ref="A39:A50"/>
+    <mergeCell ref="A51:A62"/>
+    <mergeCell ref="A63:A74"/>
+    <mergeCell ref="A75:A86"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:A14"/>
     <mergeCell ref="A15:A26"/>
-    <mergeCell ref="A27:A38"/>
-    <mergeCell ref="A39:A50"/>
-    <mergeCell ref="A51:A62"/>
-    <mergeCell ref="A63:A74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Python medium done, rust done, python high all that's left
</commit_message>
<xml_diff>
--- a/ExperimentParameters.xlsx
+++ b/ExperimentParameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monkj\CS630Project\CS630Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54AEFB8-F663-4AB2-A1E3-D53A28BAA059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4639BA7-C3F0-4082-B613-26C8C236E453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,12 +59,6 @@
     <t>High Load</t>
   </si>
   <si>
-    <t>Low Load Computation: Sum integers from 1 to n</t>
-  </si>
-  <si>
-    <t>High Load Computation: Multiply 2 nxn matrices</t>
-  </si>
-  <si>
     <t>Java</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
   </si>
   <si>
     <t>C++</t>
-  </si>
-  <si>
-    <t>Medium Load Computation: Sort n randomly generated numbers (quick sort)</t>
   </si>
   <si>
     <t>C#</t>
@@ -136,12 +127,21 @@
   <si>
     <t>Rust</t>
   </si>
+  <si>
+    <t>Low Load Computation: Sum integers from 1 to 984,600,000</t>
+  </si>
+  <si>
+    <t>Medium Load Computation: Sort 1,000,000 randomly generated numbers (quick sort)</t>
+  </si>
+  <si>
+    <t>High Load Computation: Multiply 2 2000x2000 matrices</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +163,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -390,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -407,6 +413,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -425,17 +443,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J101" sqref="J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,52 +755,52 @@
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="14" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="17"/>
+      <c r="H2" s="21"/>
       <c r="L2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="15"/>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2">
         <v>1.4410000000000001</v>
@@ -815,13 +824,13 @@
         <v>56</v>
       </c>
       <c r="L4" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2">
         <v>1.4410000000000001</v>
@@ -846,9 +855,9 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2">
         <v>1.4339999999999999</v>
@@ -872,13 +881,13 @@
         <v>38.099999999999994</v>
       </c>
       <c r="L6" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="15"/>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2">
         <v>1.4410000000000001</v>
@@ -903,9 +912,9 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="15"/>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2">
         <v>1.4359999999999999</v>
@@ -930,9 +939,9 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="15"/>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2">
         <v>1.4510000000000001</v>
@@ -956,13 +965,13 @@
         <v>39.700000000000003</v>
       </c>
       <c r="L9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="15"/>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2">
         <v>1.4279999999999999</v>
@@ -989,13 +998,13 @@
         <v>58</v>
       </c>
       <c r="M10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="15"/>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2">
         <v>1.4419999999999999</v>
@@ -1019,13 +1028,13 @@
         <v>39.200000000000003</v>
       </c>
       <c r="L11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="15"/>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2">
         <v>1.4350000000000001</v>
@@ -1050,9 +1059,9 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C13" s="3">
         <v>1.4339999999999999</v>
@@ -1077,9 +1086,9 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" ref="C14:H14" si="0">AVERAGE(C4:C13)</f>
@@ -1107,35 +1116,35 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
-        <v>9</v>
+      <c r="A15" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>3</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="15"/>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2">
         <v>0.21199999999999999</v>
@@ -1160,9 +1169,9 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="15"/>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2">
         <v>0.20699999999999999</v>
@@ -1187,9 +1196,9 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="15"/>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2">
         <v>0.20599999999999999</v>
@@ -1214,9 +1223,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="15"/>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2">
         <v>0.214</v>
@@ -1241,9 +1250,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="15"/>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2">
         <v>0.21099999999999999</v>
@@ -1268,9 +1277,9 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
+      <c r="A21" s="15"/>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C21" s="2">
         <v>0.20499999999999999</v>
@@ -1295,9 +1304,9 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
+      <c r="A22" s="15"/>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C22" s="2">
         <v>0.21199999999999999</v>
@@ -1322,9 +1331,9 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
+      <c r="A23" s="15"/>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2">
         <v>0.20699999999999999</v>
@@ -1349,9 +1358,9 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+      <c r="A24" s="15"/>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C24" s="2">
         <v>0.20499999999999999</v>
@@ -1376,9 +1385,9 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C25" s="3">
         <v>0.20599999999999999</v>
@@ -1403,9 +1412,9 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" ref="C26:H26" si="1">AVERAGE(C16:C25)</f>
@@ -1433,35 +1442,35 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
-        <v>19</v>
+      <c r="A27" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>3</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
+      <c r="A28" s="15"/>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C28" s="2">
         <v>0.38900000000000001</v>
@@ -1486,9 +1495,9 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
+      <c r="A29" s="15"/>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C29" s="2">
         <v>0.39900000000000002</v>
@@ -1513,9 +1522,9 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
+      <c r="A30" s="15"/>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C30" s="2">
         <v>0.38900000000000001</v>
@@ -1540,9 +1549,9 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="A31" s="15"/>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C31" s="2">
         <v>0.39700000000000002</v>
@@ -1567,9 +1576,9 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="A32" s="15"/>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C32" s="2">
         <v>0.39400000000000002</v>
@@ -1594,9 +1603,9 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
+      <c r="A33" s="15"/>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C33" s="2">
         <v>0.39200000000000002</v>
@@ -1621,9 +1630,9 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
+      <c r="A34" s="15"/>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C34" s="2">
         <v>0.39800000000000002</v>
@@ -1648,9 +1657,9 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
+      <c r="A35" s="15"/>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C35" s="2">
         <v>0.39200000000000002</v>
@@ -1675,9 +1684,9 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
+      <c r="A36" s="15"/>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C36" s="2">
         <v>0.38900000000000001</v>
@@ -1702,9 +1711,9 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="21"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C37" s="3">
         <v>0.39500000000000002</v>
@@ -1729,9 +1738,9 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="22"/>
+      <c r="A38" s="16"/>
       <c r="B38" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" ref="C38:H38" si="2">AVERAGE(C28:C37)</f>
@@ -1759,35 +1768,35 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="20" t="s">
-        <v>10</v>
+      <c r="A39" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>3</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
+      <c r="A40" s="15"/>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C40" s="2">
         <v>18.312999999999999</v>
@@ -1807,9 +1816,9 @@
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
+      <c r="A41" s="15"/>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C41" s="2">
         <v>18.530999999999999</v>
@@ -1829,9 +1838,9 @@
       <c r="H41" s="6"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
+      <c r="A42" s="15"/>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C42" s="2">
         <v>18.297000000000001</v>
@@ -1840,15 +1849,20 @@
         <f>111.5-L10</f>
         <v>53.5</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="6"/>
+      <c r="E42" s="2">
+        <v>391.57799999999997</v>
+      </c>
+      <c r="F42" s="6">
+        <f>115.5-L10</f>
+        <v>57.5</v>
+      </c>
       <c r="G42" s="2"/>
       <c r="H42" s="6"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
+      <c r="A43" s="15"/>
       <c r="B43" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C43" s="2">
         <v>18.530999999999999</v>
@@ -1857,15 +1871,20 @@
         <f>111.4-L10</f>
         <v>53.400000000000006</v>
       </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="6"/>
+      <c r="E43" s="2">
+        <v>393.89100000000002</v>
+      </c>
+      <c r="F43" s="6">
+        <f>138.7-L10</f>
+        <v>80.699999999999989</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="6"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
+      <c r="A44" s="15"/>
       <c r="B44" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C44" s="2">
         <v>18.405999999999999</v>
@@ -1874,15 +1893,20 @@
         <f>108.8-L10</f>
         <v>50.8</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="6"/>
+      <c r="E44" s="2">
+        <v>393.68799999999999</v>
+      </c>
+      <c r="F44" s="6">
+        <f>138.9-L10</f>
+        <v>80.900000000000006</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="6"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
+      <c r="A45" s="15"/>
       <c r="B45" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C45" s="2">
         <v>18.312999999999999</v>
@@ -1891,15 +1915,20 @@
         <f>111-L10</f>
         <v>53</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="6"/>
+      <c r="E45" s="2">
+        <v>393.17200000000003</v>
+      </c>
+      <c r="F45" s="6">
+        <f>139.4-L10</f>
+        <v>81.400000000000006</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="6"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
+      <c r="A46" s="15"/>
       <c r="B46" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C46" s="2">
         <v>18.469000000000001</v>
@@ -1908,15 +1937,20 @@
         <f>107.2-L10</f>
         <v>49.2</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="6"/>
+      <c r="E46" s="2">
+        <v>390.54700000000003</v>
+      </c>
+      <c r="F46" s="6">
+        <f>127.6-L10</f>
+        <v>69.599999999999994</v>
+      </c>
       <c r="G46" s="2"/>
       <c r="H46" s="6"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
+      <c r="A47" s="15"/>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C47" s="2">
         <v>18.390999999999998</v>
@@ -1925,15 +1959,20 @@
         <f>108.4-L10</f>
         <v>50.400000000000006</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="6"/>
+      <c r="E47" s="2">
+        <v>392.15600000000001</v>
+      </c>
+      <c r="F47" s="6">
+        <f>123.8-L10</f>
+        <v>65.8</v>
+      </c>
       <c r="G47" s="2"/>
       <c r="H47" s="6"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
+      <c r="A48" s="15"/>
       <c r="B48" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C48" s="2">
         <v>18.375</v>
@@ -1942,15 +1981,20 @@
         <f>108.8-L10</f>
         <v>50.8</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="6"/>
+      <c r="E48" s="2">
+        <v>392.375</v>
+      </c>
+      <c r="F48" s="6">
+        <f>137.1-L10</f>
+        <v>79.099999999999994</v>
+      </c>
       <c r="G48" s="2"/>
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="21"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C49" s="3">
         <v>18.359000000000002</v>
@@ -1959,15 +2003,20 @@
         <f>112.5-L10</f>
         <v>54.5</v>
       </c>
-      <c r="E49" s="3"/>
-      <c r="F49" s="7"/>
+      <c r="E49" s="3">
+        <v>392.53100000000001</v>
+      </c>
+      <c r="F49" s="7">
+        <f>123.3-L10</f>
+        <v>65.3</v>
+      </c>
       <c r="G49" s="3"/>
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="22"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C50" s="1">
         <f>AVERAGE(C40:C49)</f>
@@ -1977,41 +2026,47 @@
         <f>AVERAGE(D40:D49)</f>
         <v>51.4</v>
       </c>
-      <c r="E50" s="12"/>
-      <c r="F50" s="13"/>
+      <c r="E50" s="12">
+        <f>AVERAGE(E40:E49)</f>
+        <v>391.94380000000001</v>
+      </c>
+      <c r="F50" s="13">
+        <f>AVERAGE(F40:F49)</f>
+        <v>72.209999999999994</v>
+      </c>
       <c r="G50" s="12"/>
       <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="20" t="s">
-        <v>11</v>
+      <c r="A51" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>3</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
+      <c r="A52" s="15"/>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C52" s="2">
         <v>1.446</v>
@@ -2036,9 +2091,9 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="21"/>
+      <c r="A53" s="15"/>
       <c r="B53" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C53" s="2">
         <v>1.4419999999999999</v>
@@ -2063,9 +2118,9 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="21"/>
+      <c r="A54" s="15"/>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C54" s="2">
         <v>1.44</v>
@@ -2090,9 +2145,9 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="21"/>
+      <c r="A55" s="15"/>
       <c r="B55" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C55" s="2">
         <v>1.444</v>
@@ -2117,9 +2172,9 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="21"/>
+      <c r="A56" s="15"/>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C56" s="2">
         <v>1.45</v>
@@ -2144,9 +2199,9 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="21"/>
+      <c r="A57" s="15"/>
       <c r="B57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C57" s="2">
         <v>1.4510000000000001</v>
@@ -2171,9 +2226,9 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="21"/>
+      <c r="A58" s="15"/>
       <c r="B58" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C58" s="2">
         <v>1.4450000000000001</v>
@@ -2198,9 +2253,9 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="21"/>
+      <c r="A59" s="15"/>
       <c r="B59" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C59" s="2">
         <v>1.4419999999999999</v>
@@ -2225,9 +2280,9 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="21"/>
+      <c r="A60" s="15"/>
       <c r="B60" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C60" s="2">
         <v>1.444</v>
@@ -2252,9 +2307,9 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="21"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C61" s="3">
         <v>1.4370000000000001</v>
@@ -2279,9 +2334,9 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="23"/>
+      <c r="A62" s="17"/>
       <c r="B62" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C62" s="1">
         <f t="shared" ref="C62:H62" si="3">AVERAGE(C52:C61)</f>
@@ -2309,35 +2364,35 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="20" t="s">
-        <v>13</v>
+      <c r="A63" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G63" s="8" t="s">
         <v>3</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="21"/>
+      <c r="A64" s="15"/>
       <c r="B64" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C64" s="2">
         <v>0.58399999999999996</v>
@@ -2362,9 +2417,9 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="21"/>
+      <c r="A65" s="15"/>
       <c r="B65" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C65" s="2">
         <v>0.58599999999999997</v>
@@ -2389,9 +2444,9 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="21"/>
+      <c r="A66" s="15"/>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C66" s="2">
         <v>0.59099999999999997</v>
@@ -2416,9 +2471,9 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="21"/>
+      <c r="A67" s="15"/>
       <c r="B67" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C67" s="2">
         <v>0.59</v>
@@ -2443,9 +2498,9 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="21"/>
+      <c r="A68" s="15"/>
       <c r="B68" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C68" s="2">
         <v>0.57199999999999995</v>
@@ -2470,9 +2525,9 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="21"/>
+      <c r="A69" s="15"/>
       <c r="B69" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C69" s="2">
         <v>0.58299999999999996</v>
@@ -2497,9 +2552,9 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
+      <c r="A70" s="15"/>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C70" s="2">
         <v>0.58699999999999997</v>
@@ -2524,9 +2579,9 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="21"/>
+      <c r="A71" s="15"/>
       <c r="B71" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C71" s="2">
         <v>0.58699999999999997</v>
@@ -2551,9 +2606,9 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="21"/>
+      <c r="A72" s="15"/>
       <c r="B72" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C72" s="2">
         <v>0.58399999999999996</v>
@@ -2578,9 +2633,9 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="21"/>
+      <c r="A73" s="15"/>
       <c r="B73" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C73" s="3">
         <v>0.58199999999999996</v>
@@ -2605,9 +2660,9 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="22"/>
+      <c r="A74" s="16"/>
       <c r="B74" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C74" s="1">
         <f t="shared" ref="C74:H74" si="4">AVERAGE(C64:C73)</f>
@@ -2635,35 +2690,35 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="20" t="s">
-        <v>31</v>
+      <c r="A75" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G75" s="8" t="s">
         <v>3</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="21"/>
+      <c r="A76" s="15"/>
       <c r="B76" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C76" s="2">
         <v>0.19500000000000001</v>
@@ -2688,9 +2743,9 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="21"/>
+      <c r="A77" s="15"/>
       <c r="B77" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C77" s="2">
         <v>0.19700000000000001</v>
@@ -2715,9 +2770,9 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="21"/>
+      <c r="A78" s="15"/>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C78" s="2">
         <v>0.19400000000000001</v>
@@ -2742,9 +2797,9 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="21"/>
+      <c r="A79" s="15"/>
       <c r="B79" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C79" s="2">
         <v>0.19500000000000001</v>
@@ -2769,9 +2824,9 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="21"/>
+      <c r="A80" s="15"/>
       <c r="B80" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C80" s="2">
         <v>0.19900000000000001</v>
@@ -2796,9 +2851,9 @@
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="21"/>
+      <c r="A81" s="15"/>
       <c r="B81" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C81" s="2">
         <v>0.19700000000000001</v>
@@ -2823,9 +2878,9 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="21"/>
+      <c r="A82" s="15"/>
       <c r="B82" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C82" s="2">
         <v>0.19700000000000001</v>
@@ -2850,9 +2905,9 @@
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="21"/>
+      <c r="A83" s="15"/>
       <c r="B83" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C83" s="2">
         <v>0.19800000000000001</v>
@@ -2877,9 +2932,9 @@
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="21"/>
+      <c r="A84" s="15"/>
       <c r="B84" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C84" s="2">
         <v>0.19500000000000001</v>
@@ -2904,9 +2959,9 @@
       </c>
     </row>
     <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="21"/>
+      <c r="A85" s="15"/>
       <c r="B85" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C85" s="3">
         <v>0.19800000000000001</v>
@@ -2931,206 +2986,374 @@
       </c>
     </row>
     <row r="86" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="22"/>
+      <c r="A86" s="16"/>
       <c r="B86" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C86" s="1">
-        <f>AVERAGE(C76:C85)</f>
+        <f t="shared" ref="C86:H86" si="5">AVERAGE(C76:C85)</f>
         <v>0.19650000000000004</v>
       </c>
       <c r="D86" s="13">
-        <f>AVERAGE(D76:D85)</f>
+        <f t="shared" si="5"/>
         <v>16.310000000000002</v>
       </c>
       <c r="E86" s="12">
-        <f>AVERAGE(E76:E85)</f>
+        <f t="shared" si="5"/>
         <v>17.240000000000002</v>
       </c>
       <c r="F86" s="13">
-        <f>AVERAGE(F76:F85)</f>
+        <f t="shared" si="5"/>
         <v>63.330000000000005</v>
       </c>
       <c r="G86" s="12">
-        <f>AVERAGE(G76:G85)</f>
+        <f t="shared" si="5"/>
         <v>26.371099999999995</v>
       </c>
       <c r="H86" s="13">
-        <f>AVERAGE(H76:H85)</f>
+        <f t="shared" si="5"/>
         <v>44.449999999999989</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="20" t="s">
-        <v>32</v>
+      <c r="A87" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G87" s="8" t="s">
         <v>3</v>
       </c>
       <c r="H87" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="21"/>
+      <c r="A88" s="15"/>
       <c r="B88" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88" s="2">
+        <v>2.3290000000000002</v>
+      </c>
+      <c r="D88" s="5">
+        <f>98.7-L10</f>
+        <v>40.700000000000003</v>
+      </c>
+      <c r="E88" s="24">
+        <v>37.375</v>
+      </c>
+      <c r="F88" s="5">
+        <f>106.3-L10</f>
+        <v>48.3</v>
+      </c>
+      <c r="G88" s="2">
+        <v>203.16300000000001</v>
+      </c>
+      <c r="H88" s="5">
+        <f>119.8-L10</f>
+        <v>61.8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="15"/>
+      <c r="B89" t="s">
+        <v>19</v>
+      </c>
+      <c r="C89" s="2">
+        <v>2.3180000000000001</v>
+      </c>
+      <c r="D89" s="6">
+        <f>98.6-L10</f>
+        <v>40.599999999999994</v>
+      </c>
+      <c r="E89" s="24">
+        <v>37.795999999999999</v>
+      </c>
+      <c r="F89" s="6">
+        <f>118.3-L10</f>
+        <v>60.3</v>
+      </c>
+      <c r="G89" s="2">
+        <v>193.76900000000001</v>
+      </c>
+      <c r="H89" s="6">
+        <f>122-L10</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="15"/>
+      <c r="B90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" s="2">
+        <v>2.3170000000000002</v>
+      </c>
+      <c r="D90" s="6">
+        <f>98.2-L10</f>
+        <v>40.200000000000003</v>
+      </c>
+      <c r="E90" s="2">
+        <v>37.526000000000003</v>
+      </c>
+      <c r="F90" s="6">
+        <f>119.9-L10</f>
+        <v>61.900000000000006</v>
+      </c>
+      <c r="G90" s="2">
+        <v>194.096</v>
+      </c>
+      <c r="H90" s="6">
+        <f>122-L10</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="15"/>
+      <c r="B91" t="s">
         <v>21</v>
       </c>
-      <c r="C88" s="2"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="2"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="5"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="21"/>
-      <c r="B89" t="s">
+      <c r="C91" s="2">
+        <v>2.37</v>
+      </c>
+      <c r="D91" s="6">
+        <f>108.9-L10</f>
+        <v>50.900000000000006</v>
+      </c>
+      <c r="E91" s="2">
+        <v>37.454000000000001</v>
+      </c>
+      <c r="F91" s="6">
+        <f>118.5-L10</f>
+        <v>60.5</v>
+      </c>
+      <c r="G91" s="2">
+        <v>195.07599999999999</v>
+      </c>
+      <c r="H91" s="6">
+        <f>118.2-L10</f>
+        <v>60.2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="15"/>
+      <c r="B92" t="s">
         <v>22</v>
       </c>
-      <c r="C89" s="2"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="6"/>
-      <c r="G89" s="2"/>
-      <c r="H89" s="6"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="21"/>
-      <c r="B90" t="s">
+      <c r="C92" s="2">
+        <v>2.3319999999999999</v>
+      </c>
+      <c r="D92" s="6">
+        <f>97.5-L10</f>
+        <v>39.5</v>
+      </c>
+      <c r="E92" s="2">
+        <v>37.598999999999997</v>
+      </c>
+      <c r="F92" s="6">
+        <f>118.8-L10</f>
+        <v>60.8</v>
+      </c>
+      <c r="G92" s="2">
+        <v>193.98500000000001</v>
+      </c>
+      <c r="H92" s="6">
+        <f>121.2-L10</f>
+        <v>63.2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="15"/>
+      <c r="B93" t="s">
         <v>23</v>
       </c>
-      <c r="C90" s="2"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="6"/>
-      <c r="G90" s="2"/>
-      <c r="H90" s="6"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="21"/>
-      <c r="B91" t="s">
+      <c r="C93" s="2">
+        <v>2.33</v>
+      </c>
+      <c r="D93" s="6">
+        <f>98.1-L10</f>
+        <v>40.099999999999994</v>
+      </c>
+      <c r="E93" s="2">
+        <v>37.636000000000003</v>
+      </c>
+      <c r="F93" s="6">
+        <f>118.1-L10</f>
+        <v>60.099999999999994</v>
+      </c>
+      <c r="G93" s="2">
+        <v>193.54</v>
+      </c>
+      <c r="H93" s="6">
+        <f>123.1-L10</f>
+        <v>65.099999999999994</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="15"/>
+      <c r="B94" t="s">
         <v>24</v>
       </c>
-      <c r="C91" s="2"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="6"/>
-      <c r="G91" s="2"/>
-      <c r="H91" s="6"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="21"/>
-      <c r="B92" t="s">
+      <c r="C94" s="2">
+        <v>2.319</v>
+      </c>
+      <c r="D94" s="6">
+        <f>97.9-L10</f>
+        <v>39.900000000000006</v>
+      </c>
+      <c r="E94" s="2">
+        <v>37.624000000000002</v>
+      </c>
+      <c r="F94" s="6">
+        <f>102-L10</f>
+        <v>44</v>
+      </c>
+      <c r="G94" s="2">
+        <v>193.65100000000001</v>
+      </c>
+      <c r="H94" s="6">
+        <f>120.8-L10</f>
+        <v>62.8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="15"/>
+      <c r="B95" t="s">
         <v>25</v>
       </c>
-      <c r="C92" s="2"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="6"/>
-      <c r="G92" s="2"/>
-      <c r="H92" s="6"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="21"/>
-      <c r="B93" t="s">
+      <c r="C95" s="2">
+        <v>2.363</v>
+      </c>
+      <c r="D95" s="6">
+        <f>97-L10</f>
+        <v>39</v>
+      </c>
+      <c r="E95" s="2">
+        <v>37.454999999999998</v>
+      </c>
+      <c r="F95" s="6">
+        <f>120-L10</f>
+        <v>62</v>
+      </c>
+      <c r="G95" s="2">
+        <v>192.71600000000001</v>
+      </c>
+      <c r="H95" s="6">
+        <f>104.6-L10</f>
+        <v>46.599999999999994</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="15"/>
+      <c r="B96" t="s">
         <v>26</v>
       </c>
-      <c r="C93" s="2"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="6"/>
-      <c r="G93" s="2"/>
-      <c r="H93" s="6"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="21"/>
-      <c r="B94" t="s">
+      <c r="C96" s="2">
+        <v>2.3170000000000002</v>
+      </c>
+      <c r="D96" s="6">
+        <f>99-L10</f>
+        <v>41</v>
+      </c>
+      <c r="E96" s="24">
+        <v>37.622</v>
+      </c>
+      <c r="F96" s="6">
+        <f>103.2-L10</f>
+        <v>45.2</v>
+      </c>
+      <c r="G96" s="2">
+        <v>193.46</v>
+      </c>
+      <c r="H96" s="6">
+        <f>124.1-L10</f>
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="15"/>
+      <c r="B97" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C94" s="2"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="6"/>
-      <c r="G94" s="2"/>
-      <c r="H94" s="6"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="21"/>
-      <c r="B95" t="s">
-        <v>28</v>
-      </c>
-      <c r="C95" s="2"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="6"/>
-      <c r="G95" s="2"/>
-      <c r="H95" s="6"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="21"/>
-      <c r="B96" t="s">
-        <v>29</v>
-      </c>
-      <c r="C96" s="2"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="6"/>
-      <c r="G96" s="2"/>
-      <c r="H96" s="6"/>
-    </row>
-    <row r="97" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="21"/>
-      <c r="B97" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C97" s="3"/>
-      <c r="D97" s="7"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="7"/>
-      <c r="G97" s="3"/>
-      <c r="H97" s="7"/>
+      <c r="C97" s="3">
+        <v>2.3490000000000002</v>
+      </c>
+      <c r="D97" s="7">
+        <f>98.2-L10</f>
+        <v>40.200000000000003</v>
+      </c>
+      <c r="E97" s="3">
+        <v>37.447000000000003</v>
+      </c>
+      <c r="F97" s="7">
+        <f>119.1-L10</f>
+        <v>61.099999999999994</v>
+      </c>
+      <c r="G97" s="3">
+        <v>193.51400000000001</v>
+      </c>
+      <c r="H97" s="7">
+        <f>120.8-L10</f>
+        <v>62.8</v>
+      </c>
     </row>
     <row r="98" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="22"/>
+      <c r="A98" s="16"/>
       <c r="B98" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C98" s="1"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="13"/>
+        <v>17</v>
+      </c>
+      <c r="C98" s="1">
+        <f>AVERAGE(C88:C97)</f>
+        <v>2.3344</v>
+      </c>
+      <c r="D98" s="13">
+        <f>AVERAGE(D88:D97)</f>
+        <v>41.209999999999994</v>
+      </c>
+      <c r="E98" s="12">
+        <f>AVERAGE(E88:E97)</f>
+        <v>37.553399999999996</v>
+      </c>
+      <c r="F98" s="13">
+        <f>AVERAGE(F88:F97)</f>
+        <v>56.419999999999995</v>
+      </c>
+      <c r="G98" s="12">
+        <f>AVERAGE(G88:G97)</f>
+        <v>194.69700000000003</v>
+      </c>
+      <c r="H98" s="13">
+        <f>AVERAGE(H88:H97)</f>
+        <v>61.659999999999989</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A15:A26"/>
     <mergeCell ref="A87:A98"/>
     <mergeCell ref="A27:A38"/>
     <mergeCell ref="A39:A50"/>
     <mergeCell ref="A51:A62"/>
     <mergeCell ref="A63:A74"/>
     <mergeCell ref="A75:A86"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:A14"/>
-    <mergeCell ref="A15:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>